<commit_message>
(addedd task of GREPLEN)
</commit_message>
<xml_diff>
--- a/output/OUTPUT4_A01.xlsx
+++ b/output/OUTPUT4_A01.xlsx
@@ -66,7 +66,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -129,6 +129,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -141,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -193,7 +213,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -203,7 +232,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -603,16 +638,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD33"/>
+  <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="7" customWidth="1" style="19" min="1" max="2"/>
+    <col width="7" customWidth="1" min="1" max="2"/>
     <col width="22.81640625" customWidth="1" style="1" min="3" max="30"/>
   </cols>
   <sheetData>
@@ -708,8 +743,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="16" t="inlineStr">
+    <row r="2" ht="14.5" customHeight="1">
+      <c r="A2" s="19" t="inlineStr">
         <is>
           <t>L
 E
@@ -860,7 +895,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="17" t="n"/>
+      <c r="A3" s="21" t="n"/>
       <c r="B3" s="16" t="n"/>
       <c r="C3" s="5" t="n"/>
       <c r="D3" s="5" t="n"/>
@@ -892,7 +927,7 @@
       <c r="AD3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="17" t="n"/>
+      <c r="A4" s="21" t="n"/>
       <c r="B4" s="16" t="inlineStr">
         <is>
           <t>F</t>
@@ -1032,18 +1067,30 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="17" t="n"/>
+      <c r="A5" s="21" t="n"/>
       <c r="B5" s="16" t="n"/>
       <c r="C5" s="5" t="n"/>
       <c r="D5" s="5" t="n"/>
       <c r="E5" s="2" t="n"/>
       <c r="F5" s="7" t="n"/>
-      <c r="G5" s="7" t="n"/>
+      <c r="G5" s="22" t="inlineStr">
+        <is>
+          <t>RW200254-</t>
+        </is>
+      </c>
       <c r="H5" s="7" t="n"/>
-      <c r="I5" s="7" t="n"/>
+      <c r="I5" s="22" t="inlineStr">
+        <is>
+          <t>RW200202-</t>
+        </is>
+      </c>
       <c r="J5" s="7" t="n"/>
       <c r="K5" s="7" t="n"/>
-      <c r="L5" s="7" t="n"/>
+      <c r="L5" s="22" t="inlineStr">
+        <is>
+          <t>RW200157-</t>
+        </is>
+      </c>
       <c r="M5" s="7" t="n"/>
       <c r="N5" s="7" t="n"/>
       <c r="O5" s="7" t="n"/>
@@ -1055,7 +1102,11 @@
       <c r="U5" s="7" t="n"/>
       <c r="V5" s="7" t="n"/>
       <c r="W5" s="7" t="n"/>
-      <c r="X5" s="7" t="n"/>
+      <c r="X5" s="22" t="inlineStr">
+        <is>
+          <t>RW200037-</t>
+        </is>
+      </c>
       <c r="Y5" s="7" t="n"/>
       <c r="Z5" s="7" t="n"/>
       <c r="AA5" s="7" t="n"/>
@@ -1064,7 +1115,7 @@
       <c r="AD5" s="7" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="17" t="n"/>
+      <c r="A6" s="21" t="n"/>
       <c r="B6" s="16" t="inlineStr">
         <is>
           <t>E</t>
@@ -1204,30 +1255,50 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="17" t="n"/>
+      <c r="A7" s="21" t="n"/>
       <c r="B7" s="16" t="n"/>
       <c r="C7" s="5" t="n"/>
       <c r="D7" s="5" t="n"/>
       <c r="E7" s="2" t="n"/>
       <c r="F7" s="7" t="n"/>
-      <c r="G7" s="7" t="n"/>
+      <c r="G7" s="22" t="inlineStr">
+        <is>
+          <t>RW200211-</t>
+        </is>
+      </c>
       <c r="H7" s="7" t="n"/>
       <c r="I7" s="7" t="n"/>
-      <c r="J7" s="7" t="n"/>
-      <c r="K7" s="7" t="n"/>
+      <c r="J7" s="22" t="inlineStr">
+        <is>
+          <t>RW200272-</t>
+        </is>
+      </c>
+      <c r="K7" s="22" t="inlineStr">
+        <is>
+          <t>RW200206-</t>
+        </is>
+      </c>
       <c r="L7" s="7" t="n"/>
       <c r="M7" s="7" t="n"/>
       <c r="N7" s="7" t="n"/>
       <c r="O7" s="7" t="n"/>
       <c r="P7" s="7" t="n"/>
-      <c r="Q7" s="7" t="n"/>
+      <c r="Q7" s="22" t="inlineStr">
+        <is>
+          <t>RW200308-</t>
+        </is>
+      </c>
       <c r="R7" s="7" t="n"/>
       <c r="S7" s="7" t="n"/>
       <c r="T7" s="7" t="n"/>
       <c r="U7" s="7" t="n"/>
       <c r="V7" s="7" t="n"/>
       <c r="W7" s="7" t="n"/>
-      <c r="X7" s="7" t="n"/>
+      <c r="X7" s="22" t="inlineStr">
+        <is>
+          <t>RW200212-</t>
+        </is>
+      </c>
       <c r="Y7" s="7" t="n"/>
       <c r="Z7" s="7" t="n"/>
       <c r="AA7" s="7" t="n"/>
@@ -1236,7 +1307,7 @@
       <c r="AD7" s="7" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="17" t="n"/>
+      <c r="A8" s="21" t="n"/>
       <c r="B8" s="16" t="inlineStr">
         <is>
           <t>D</t>
@@ -1376,7 +1447,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="17" t="n"/>
+      <c r="A9" s="21" t="n"/>
       <c r="B9" s="16" t="n"/>
       <c r="C9" s="5" t="n"/>
       <c r="D9" s="5" t="n"/>
@@ -1408,7 +1479,7 @@
       <c r="AD9" s="7" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="17" t="n"/>
+      <c r="A10" s="21" t="n"/>
       <c r="B10" s="16" t="inlineStr">
         <is>
           <t>C</t>
@@ -1548,7 +1619,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="n"/>
+      <c r="A11" s="21" t="n"/>
       <c r="B11" s="16" t="n"/>
       <c r="C11" s="5" t="n"/>
       <c r="D11" s="5" t="n"/>
@@ -1580,7 +1651,7 @@
       <c r="AD11" s="7" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="17" t="n"/>
+      <c r="A12" s="21" t="n"/>
       <c r="B12" s="16" t="inlineStr">
         <is>
           <t>B</t>
@@ -1720,7 +1791,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="18" t="n"/>
+      <c r="A13" s="21" t="n"/>
       <c r="B13" s="16" t="n"/>
       <c r="C13" s="13" t="n"/>
       <c r="D13" s="13" t="n"/>
@@ -1752,6 +1823,7 @@
       <c r="AD13" s="13" t="n"/>
     </row>
     <row r="14">
+      <c r="A14" s="21" t="n"/>
       <c r="B14" s="16" t="inlineStr">
         <is>
           <t>A</t>
@@ -1890,7 +1962,8 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="21.5" customHeight="1" s="19">
+    <row r="15" ht="21.5" customHeight="1">
+      <c r="A15" s="21" t="n"/>
       <c r="B15" s="16" t="n"/>
       <c r="C15" s="5" t="n"/>
       <c r="D15" s="5" t="n"/>
@@ -1921,7 +1994,7 @@
       <c r="AC15" s="3" t="n"/>
       <c r="AD15" s="3" t="n"/>
     </row>
-    <row r="16" ht="17" customHeight="1" s="19">
+    <row r="16" ht="17" customHeight="1">
       <c r="A16" s="6" t="n"/>
       <c r="B16" s="6" t="n"/>
       <c r="C16" s="6" t="inlineStr">
@@ -2337,21 +2410,41 @@
       <c r="Q19" s="8" t="n"/>
       <c r="R19" s="8" t="n"/>
       <c r="S19" s="8" t="n"/>
-      <c r="T19" s="8" t="n"/>
-      <c r="U19" s="8" t="n"/>
-      <c r="V19" s="8" t="n"/>
+      <c r="T19" s="23" t="inlineStr">
+        <is>
+          <t>B2000305-</t>
+        </is>
+      </c>
+      <c r="U19" s="23" t="inlineStr">
+        <is>
+          <t>b1000287-</t>
+        </is>
+      </c>
+      <c r="V19" s="23" t="inlineStr">
+        <is>
+          <t>B2011065-</t>
+        </is>
+      </c>
       <c r="W19" s="8" t="n"/>
       <c r="X19" s="8" t="n"/>
-      <c r="Y19" s="8" t="n"/>
+      <c r="Y19" s="23" t="inlineStr">
+        <is>
+          <t>b1007311-</t>
+        </is>
+      </c>
       <c r="Z19" s="8" t="n"/>
       <c r="AA19" s="8" t="n"/>
-      <c r="AB19" s="20" t="inlineStr">
+      <c r="AB19" s="23" t="inlineStr">
         <is>
           <t>B1007919-</t>
         </is>
       </c>
       <c r="AC19" s="8" t="n"/>
-      <c r="AD19" s="8" t="n"/>
+      <c r="AD19" s="23" t="inlineStr">
+        <is>
+          <t>b2000660-</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="17" t="n"/>
@@ -2504,120 +2597,131 @@
     <row r="21">
       <c r="A21" s="17" t="n"/>
       <c r="B21" s="16" t="n"/>
-      <c r="C21" s="20" t="inlineStr">
+      <c r="C21" s="23" t="inlineStr">
         <is>
           <t>B2010530-</t>
         </is>
       </c>
-      <c r="D21" s="8" t="n"/>
-      <c r="E21" s="20" t="inlineStr">
+      <c r="D21" s="23" t="inlineStr">
+        <is>
+          <t>B2010464-</t>
+        </is>
+      </c>
+      <c r="E21" s="23" t="inlineStr">
         <is>
           <t>b1000323-</t>
         </is>
       </c>
-      <c r="F21" s="20" t="inlineStr">
+      <c r="F21" s="23" t="inlineStr">
         <is>
           <t>b1000309-</t>
         </is>
       </c>
-      <c r="G21" s="20" t="inlineStr">
+      <c r="G21" s="23" t="inlineStr">
         <is>
           <t>B2011272-</t>
         </is>
       </c>
-      <c r="H21" s="20" t="inlineStr">
+      <c r="H21" s="23" t="inlineStr">
         <is>
           <t>B1006102-</t>
         </is>
       </c>
-      <c r="I21" s="20" t="inlineStr">
+      <c r="I21" s="23" t="inlineStr">
         <is>
           <t>B2010532-</t>
         </is>
       </c>
-      <c r="J21" s="20" t="inlineStr">
+      <c r="J21" s="23" t="inlineStr">
         <is>
           <t>B2010512-</t>
         </is>
       </c>
-      <c r="K21" s="20" t="inlineStr">
-        <is>
-          <t>B1006735-</t>
+      <c r="K21" s="23" t="inlineStr">
+        <is>
+          <t>B2010465-</t>
         </is>
       </c>
       <c r="L21" s="8" t="n"/>
-      <c r="M21" s="20" t="inlineStr">
+      <c r="M21" s="23" t="inlineStr">
         <is>
           <t>m1017659-</t>
         </is>
       </c>
-      <c r="N21" s="20" t="inlineStr">
+      <c r="N21" s="23" t="inlineStr">
         <is>
           <t>B1000313-</t>
         </is>
       </c>
-      <c r="O21" s="20" t="inlineStr">
-        <is>
-          <t>B1006176-</t>
-        </is>
-      </c>
-      <c r="P21" s="8" t="n"/>
-      <c r="Q21" s="8" t="n"/>
-      <c r="R21" s="21" t="inlineStr">
-        <is>
-          <t>B2010458-
-B2011122-</t>
-        </is>
-      </c>
-      <c r="S21" s="20" t="inlineStr">
-        <is>
-          <t>B2010156-</t>
-        </is>
-      </c>
-      <c r="T21" s="20" t="inlineStr">
+      <c r="O21" s="8" t="n"/>
+      <c r="P21" s="23" t="inlineStr">
+        <is>
+          <t>b2011489-</t>
+        </is>
+      </c>
+      <c r="Q21" s="23" t="inlineStr">
+        <is>
+          <t>B2010458-</t>
+        </is>
+      </c>
+      <c r="R21" s="8" t="n"/>
+      <c r="S21" s="23" t="inlineStr">
+        <is>
+          <t>B1008877-</t>
+        </is>
+      </c>
+      <c r="T21" s="23" t="inlineStr">
         <is>
           <t>B1004997-</t>
         </is>
       </c>
-      <c r="U21" s="20" t="inlineStr">
+      <c r="U21" s="23" t="inlineStr">
         <is>
           <t>B2011290-</t>
         </is>
       </c>
-      <c r="V21" s="8" t="n"/>
-      <c r="W21" s="20" t="inlineStr">
+      <c r="V21" s="23" t="inlineStr">
+        <is>
+          <t>P1209364-</t>
+        </is>
+      </c>
+      <c r="W21" s="23" t="inlineStr">
         <is>
           <t>p1234159-</t>
         </is>
       </c>
-      <c r="X21" s="20" t="inlineStr">
+      <c r="X21" s="23" t="inlineStr">
         <is>
           <t>B2011317-</t>
         </is>
       </c>
-      <c r="Y21" s="20" t="inlineStr">
-        <is>
-          <t>B2011062-</t>
-        </is>
-      </c>
-      <c r="Z21" s="20" t="inlineStr">
+      <c r="Y21" s="23" t="inlineStr">
+        <is>
+          <t>B2011491-</t>
+        </is>
+      </c>
+      <c r="Z21" s="23" t="inlineStr">
         <is>
           <t>B2000859-</t>
         </is>
       </c>
-      <c r="AA21" s="8" t="n"/>
-      <c r="AB21" s="20" t="inlineStr">
+      <c r="AA21" s="23" t="inlineStr">
+        <is>
+          <t>B1006183-</t>
+        </is>
+      </c>
+      <c r="AB21" s="23" t="inlineStr">
         <is>
           <t>B2011283-</t>
         </is>
       </c>
-      <c r="AC21" s="21" t="inlineStr">
+      <c r="AC21" s="24" t="inlineStr">
         <is>
           <t>B2011308-
 P1229403-</t>
         </is>
       </c>
-      <c r="AD21" s="20" t="inlineStr">
+      <c r="AD21" s="23" t="inlineStr">
         <is>
           <t>B1008952-</t>
         </is>
@@ -2774,110 +2878,142 @@
     <row r="23">
       <c r="A23" s="17" t="n"/>
       <c r="B23" s="16" t="n"/>
-      <c r="C23" s="8" t="n"/>
-      <c r="D23" s="20" t="inlineStr">
+      <c r="C23" s="23" t="inlineStr">
+        <is>
+          <t>B1008831-</t>
+        </is>
+      </c>
+      <c r="D23" s="23" t="inlineStr">
         <is>
           <t>t2001237-</t>
         </is>
       </c>
-      <c r="E23" s="8" t="n"/>
-      <c r="F23" s="20" t="inlineStr">
+      <c r="E23" s="23" t="inlineStr">
+        <is>
+          <t>B2010925-</t>
+        </is>
+      </c>
+      <c r="F23" s="23" t="inlineStr">
         <is>
           <t>B2010514-</t>
         </is>
       </c>
-      <c r="G23" s="20" t="inlineStr">
+      <c r="G23" s="23" t="inlineStr">
         <is>
           <t>b1004719-</t>
         </is>
       </c>
-      <c r="H23" s="8" t="n"/>
-      <c r="I23" s="8" t="n"/>
-      <c r="J23" s="20" t="inlineStr">
+      <c r="H23" s="23" t="inlineStr">
+        <is>
+          <t>b2009951-</t>
+        </is>
+      </c>
+      <c r="I23" s="23" t="inlineStr">
+        <is>
+          <t>P1227414-</t>
+        </is>
+      </c>
+      <c r="J23" s="23" t="inlineStr">
         <is>
           <t>M1012367-</t>
         </is>
       </c>
-      <c r="K23" s="20" t="inlineStr">
+      <c r="K23" s="23" t="inlineStr">
         <is>
           <t>B2010521-</t>
         </is>
       </c>
-      <c r="L23" s="20" t="inlineStr">
-        <is>
-          <t>b1007931-</t>
-        </is>
-      </c>
-      <c r="M23" s="20" t="inlineStr">
+      <c r="L23" s="23" t="inlineStr">
+        <is>
+          <t>B2012313-</t>
+        </is>
+      </c>
+      <c r="M23" s="23" t="inlineStr">
         <is>
           <t>b2010463-</t>
         </is>
       </c>
-      <c r="N23" s="20" t="inlineStr">
+      <c r="N23" s="23" t="inlineStr">
         <is>
           <t>b2000081-</t>
         </is>
       </c>
-      <c r="O23" s="8" t="n"/>
-      <c r="P23" s="20" t="inlineStr">
-        <is>
-          <t>A1002450-</t>
-        </is>
-      </c>
-      <c r="Q23" s="20" t="inlineStr">
+      <c r="O23" s="23" t="inlineStr">
+        <is>
+          <t>B2010111-</t>
+        </is>
+      </c>
+      <c r="P23" s="23" t="inlineStr">
+        <is>
+          <t>B2000018-</t>
+        </is>
+      </c>
+      <c r="Q23" s="23" t="inlineStr">
+        <is>
+          <t>B2011500-</t>
+        </is>
+      </c>
+      <c r="R23" s="23" t="inlineStr">
         <is>
           <t>B2000933-</t>
         </is>
       </c>
-      <c r="R23" s="8" t="n"/>
-      <c r="S23" s="8" t="n"/>
-      <c r="T23" s="8" t="n"/>
-      <c r="U23" s="20" t="inlineStr">
+      <c r="S23" s="23" t="inlineStr">
+        <is>
+          <t>B1009009-</t>
+        </is>
+      </c>
+      <c r="T23" s="23" t="inlineStr">
+        <is>
+          <t>X1000258-</t>
+        </is>
+      </c>
+      <c r="U23" s="23" t="inlineStr">
         <is>
           <t>B2011297-</t>
         </is>
       </c>
-      <c r="V23" s="20" t="inlineStr">
+      <c r="V23" s="23" t="inlineStr">
         <is>
           <t>B2010874-</t>
         </is>
       </c>
-      <c r="W23" s="20" t="inlineStr">
+      <c r="W23" s="23" t="inlineStr">
         <is>
           <t>B1006288-</t>
         </is>
       </c>
-      <c r="X23" s="20" t="inlineStr">
-        <is>
-          <t>B2000448-</t>
-        </is>
-      </c>
-      <c r="Y23" s="20" t="inlineStr">
+      <c r="X23" s="23" t="inlineStr">
+        <is>
+          <t>B2000465-</t>
+        </is>
+      </c>
+      <c r="Y23" s="23" t="inlineStr">
         <is>
           <t>B1005034-</t>
         </is>
       </c>
-      <c r="Z23" s="20" t="inlineStr">
+      <c r="Z23" s="23" t="inlineStr">
         <is>
           <t>B2011292-</t>
         </is>
       </c>
-      <c r="AA23" s="20" t="inlineStr">
-        <is>
-          <t>B2000455-</t>
-        </is>
-      </c>
-      <c r="AB23" s="20" t="inlineStr">
+      <c r="AA23" s="23" t="inlineStr">
+        <is>
+          <t>B2011496-</t>
+        </is>
+      </c>
+      <c r="AB23" s="23" t="inlineStr">
         <is>
           <t>B2011293-</t>
         </is>
       </c>
-      <c r="AC23" s="20" t="inlineStr">
+      <c r="AC23" s="23" t="inlineStr">
         <is>
           <t>t1000756-</t>
         </is>
       </c>
-      <c r="AD23" s="20" t="inlineStr">
+      <c r="AD23" s="23" t="inlineStr">
         <is>
           <t>B1000063-</t>
         </is>
@@ -3034,118 +3170,138 @@
     <row r="25">
       <c r="A25" s="17" t="n"/>
       <c r="B25" s="16" t="n"/>
-      <c r="C25" s="20" t="inlineStr">
+      <c r="C25" s="23" t="inlineStr">
         <is>
           <t>T2000320-</t>
         </is>
       </c>
-      <c r="D25" s="20" t="inlineStr">
+      <c r="D25" s="23" t="inlineStr">
         <is>
           <t>t2001172-</t>
         </is>
       </c>
-      <c r="E25" s="20" t="inlineStr">
+      <c r="E25" s="23" t="inlineStr">
         <is>
           <t>B1006724-</t>
         </is>
       </c>
-      <c r="F25" s="20" t="inlineStr">
+      <c r="F25" s="23" t="inlineStr">
         <is>
           <t>t2001262-</t>
         </is>
       </c>
-      <c r="G25" s="20" t="inlineStr">
+      <c r="G25" s="23" t="inlineStr">
         <is>
           <t>M1013183-</t>
         </is>
       </c>
-      <c r="H25" s="20" t="inlineStr">
+      <c r="H25" s="23" t="inlineStr">
         <is>
           <t>B2010631-</t>
         </is>
       </c>
-      <c r="I25" s="8" t="n"/>
-      <c r="J25" s="20" t="inlineStr">
+      <c r="I25" s="23" t="inlineStr">
+        <is>
+          <t>T2003054-</t>
+        </is>
+      </c>
+      <c r="J25" s="23" t="inlineStr">
         <is>
           <t>B2010529-</t>
         </is>
       </c>
-      <c r="K25" s="20" t="inlineStr">
+      <c r="K25" s="23" t="inlineStr">
         <is>
           <t>M1016841-</t>
         </is>
       </c>
-      <c r="L25" s="20" t="inlineStr">
-        <is>
-          <t>b1007290-</t>
-        </is>
-      </c>
-      <c r="M25" s="20" t="inlineStr">
+      <c r="L25" s="23" t="inlineStr">
+        <is>
+          <t>B1007772-</t>
+        </is>
+      </c>
+      <c r="M25" s="23" t="inlineStr">
         <is>
           <t>B2010466-</t>
         </is>
       </c>
       <c r="N25" s="8" t="n"/>
-      <c r="O25" s="20" t="inlineStr">
+      <c r="O25" s="23" t="inlineStr">
         <is>
           <t>B2000474-</t>
         </is>
       </c>
-      <c r="P25" s="20" t="inlineStr">
+      <c r="P25" s="23" t="inlineStr">
         <is>
           <t>B2010884-</t>
         </is>
       </c>
-      <c r="Q25" s="20" t="inlineStr">
-        <is>
-          <t>B1006751-</t>
-        </is>
-      </c>
-      <c r="R25" s="8" t="n"/>
-      <c r="S25" s="20" t="inlineStr">
-        <is>
-          <t>T2001332-</t>
-        </is>
-      </c>
-      <c r="T25" s="8" t="n"/>
-      <c r="U25" s="8" t="n"/>
-      <c r="V25" s="20" t="inlineStr">
+      <c r="Q25" s="23" t="inlineStr">
+        <is>
+          <t>B2000412-</t>
+        </is>
+      </c>
+      <c r="R25" s="23" t="inlineStr">
+        <is>
+          <t>B1006465-</t>
+        </is>
+      </c>
+      <c r="S25" s="23" t="inlineStr">
+        <is>
+          <t>X1000208-</t>
+        </is>
+      </c>
+      <c r="T25" s="23" t="inlineStr">
+        <is>
+          <t>t2001958-</t>
+        </is>
+      </c>
+      <c r="U25" s="23" t="inlineStr">
+        <is>
+          <t>T2000236-</t>
+        </is>
+      </c>
+      <c r="V25" s="23" t="inlineStr">
         <is>
           <t>B2011305-</t>
         </is>
       </c>
-      <c r="W25" s="20" t="inlineStr">
+      <c r="W25" s="23" t="inlineStr">
         <is>
           <t>B2000144-</t>
         </is>
       </c>
-      <c r="X25" s="20" t="inlineStr">
+      <c r="X25" s="23" t="inlineStr">
         <is>
           <t>b2010452-</t>
         </is>
       </c>
-      <c r="Y25" s="20" t="inlineStr">
+      <c r="Y25" s="23" t="inlineStr">
         <is>
           <t>p1225708-</t>
         </is>
       </c>
-      <c r="Z25" s="8" t="n"/>
-      <c r="AA25" s="20" t="inlineStr">
-        <is>
-          <t>B2010336-</t>
-        </is>
-      </c>
-      <c r="AB25" s="20" t="inlineStr">
-        <is>
-          <t>P1204055-</t>
-        </is>
-      </c>
-      <c r="AC25" s="20" t="inlineStr">
+      <c r="Z25" s="23" t="inlineStr">
+        <is>
+          <t>t2003030-</t>
+        </is>
+      </c>
+      <c r="AA25" s="23" t="inlineStr">
+        <is>
+          <t>B2000987-</t>
+        </is>
+      </c>
+      <c r="AB25" s="23" t="inlineStr">
+        <is>
+          <t>b1007722-</t>
+        </is>
+      </c>
+      <c r="AC25" s="23" t="inlineStr">
         <is>
           <t>B2011319-</t>
         </is>
       </c>
-      <c r="AD25" s="20" t="inlineStr">
+      <c r="AD25" s="23" t="inlineStr">
         <is>
           <t>B2011306-</t>
         </is>
@@ -3302,49 +3458,53 @@
     <row r="27">
       <c r="A27" s="17" t="n"/>
       <c r="B27" s="16" t="n"/>
-      <c r="C27" s="8" t="n"/>
-      <c r="D27" s="20" t="inlineStr">
-        <is>
-          <t>B1006750-</t>
-        </is>
-      </c>
-      <c r="E27" s="20" t="inlineStr">
+      <c r="C27" s="23" t="inlineStr">
+        <is>
+          <t>T1000424-</t>
+        </is>
+      </c>
+      <c r="D27" s="23" t="inlineStr">
+        <is>
+          <t>B2012223-</t>
+        </is>
+      </c>
+      <c r="E27" s="23" t="inlineStr">
         <is>
           <t>T2000278-</t>
         </is>
       </c>
-      <c r="F27" s="20" t="inlineStr">
-        <is>
-          <t>B1004816-</t>
-        </is>
-      </c>
-      <c r="G27" s="20" t="inlineStr">
-        <is>
-          <t>t2001235-</t>
-        </is>
-      </c>
-      <c r="H27" s="20" t="inlineStr">
+      <c r="F27" s="23" t="inlineStr">
+        <is>
+          <t>B1004352-</t>
+        </is>
+      </c>
+      <c r="G27" s="23" t="inlineStr">
+        <is>
+          <t>T2003282-</t>
+        </is>
+      </c>
+      <c r="H27" s="23" t="inlineStr">
         <is>
           <t>B2010471-</t>
         </is>
       </c>
-      <c r="I27" s="20" t="inlineStr">
-        <is>
-          <t>b2010464-</t>
-        </is>
-      </c>
-      <c r="J27" s="20" t="inlineStr">
-        <is>
-          <t>B1008099-</t>
-        </is>
-      </c>
-      <c r="K27" s="20" t="inlineStr">
-        <is>
-          <t>t2001256-</t>
+      <c r="I27" s="23" t="inlineStr">
+        <is>
+          <t>B1005655-</t>
+        </is>
+      </c>
+      <c r="J27" s="23" t="inlineStr">
+        <is>
+          <t>B2000670-</t>
+        </is>
+      </c>
+      <c r="K27" s="23" t="inlineStr">
+        <is>
+          <t>b2012266-</t>
         </is>
       </c>
       <c r="L27" s="8" t="n"/>
-      <c r="M27" s="20" t="inlineStr">
+      <c r="M27" s="23" t="inlineStr">
         <is>
           <t>b2010467-</t>
         </is>
@@ -3352,62 +3512,70 @@
       <c r="N27" s="8" t="n"/>
       <c r="O27" s="8" t="n"/>
       <c r="P27" s="8" t="n"/>
-      <c r="Q27" s="8" t="n"/>
-      <c r="R27" s="8" t="n"/>
-      <c r="S27" s="20" t="inlineStr">
+      <c r="Q27" s="23" t="inlineStr">
+        <is>
+          <t>B1004679-</t>
+        </is>
+      </c>
+      <c r="R27" s="23" t="inlineStr">
+        <is>
+          <t>B2000385-</t>
+        </is>
+      </c>
+      <c r="S27" s="23" t="inlineStr">
         <is>
           <t>B1008466-</t>
         </is>
       </c>
-      <c r="T27" s="20" t="inlineStr">
-        <is>
-          <t>B1006730-</t>
-        </is>
-      </c>
-      <c r="U27" s="20" t="inlineStr">
-        <is>
-          <t>B1000287-</t>
-        </is>
-      </c>
-      <c r="V27" s="20" t="inlineStr">
-        <is>
-          <t>T2001716-</t>
-        </is>
-      </c>
-      <c r="W27" s="20" t="inlineStr">
-        <is>
-          <t>M1015375-</t>
-        </is>
-      </c>
-      <c r="X27" s="20" t="inlineStr">
+      <c r="T27" s="23" t="inlineStr">
+        <is>
+          <t>B2011497-</t>
+        </is>
+      </c>
+      <c r="U27" s="8" t="n"/>
+      <c r="V27" s="23" t="inlineStr">
+        <is>
+          <t>B2000108-</t>
+        </is>
+      </c>
+      <c r="W27" s="23" t="inlineStr">
+        <is>
+          <t>T2001399-</t>
+        </is>
+      </c>
+      <c r="X27" s="23" t="inlineStr">
         <is>
           <t>U1000142-</t>
         </is>
       </c>
-      <c r="Y27" s="20" t="inlineStr">
-        <is>
-          <t>b1007311-</t>
-        </is>
-      </c>
-      <c r="Z27" s="20" t="inlineStr">
+      <c r="Y27" s="23" t="inlineStr">
+        <is>
+          <t>B2012335-</t>
+        </is>
+      </c>
+      <c r="Z27" s="23" t="inlineStr">
         <is>
           <t>b2010469-</t>
         </is>
       </c>
-      <c r="AA27" s="20" t="inlineStr">
-        <is>
-          <t>B1008292-</t>
-        </is>
-      </c>
-      <c r="AB27" s="8" t="n"/>
-      <c r="AC27" s="20" t="inlineStr">
+      <c r="AA27" s="23" t="inlineStr">
+        <is>
+          <t>B1008343-</t>
+        </is>
+      </c>
+      <c r="AB27" s="23" t="inlineStr">
+        <is>
+          <t>T1000662-</t>
+        </is>
+      </c>
+      <c r="AC27" s="23" t="inlineStr">
         <is>
           <t>B2000449-</t>
         </is>
       </c>
-      <c r="AD27" s="20" t="inlineStr">
-        <is>
-          <t>b2000660-</t>
+      <c r="AD27" s="23" t="inlineStr">
+        <is>
+          <t>X1000262-</t>
         </is>
       </c>
     </row>
@@ -3562,114 +3730,143 @@
     <row r="29">
       <c r="A29" s="17" t="n"/>
       <c r="B29" s="16" t="n"/>
-      <c r="C29" s="22" t="inlineStr">
-        <is>
-          <t>B2011339-</t>
-        </is>
-      </c>
-      <c r="D29" s="22" t="inlineStr">
+      <c r="C29" s="25" t="inlineStr">
+        <is>
+          <t>M1015708-</t>
+        </is>
+      </c>
+      <c r="D29" s="25" t="inlineStr">
         <is>
           <t>P1222156-</t>
         </is>
       </c>
-      <c r="E29" s="14" t="n"/>
-      <c r="F29" s="22" t="inlineStr">
+      <c r="E29" s="25" t="inlineStr">
+        <is>
+          <t>B2012207-</t>
+        </is>
+      </c>
+      <c r="F29" s="25" t="inlineStr">
         <is>
           <t>B2010470-</t>
         </is>
       </c>
-      <c r="G29" s="22" t="inlineStr">
+      <c r="G29" s="25" t="inlineStr">
         <is>
           <t>B1007305-</t>
         </is>
       </c>
-      <c r="H29" s="22" t="inlineStr">
-        <is>
-          <t>B2000436-</t>
-        </is>
-      </c>
-      <c r="I29" s="22" t="inlineStr">
+      <c r="H29" s="25" t="inlineStr">
+        <is>
+          <t>M1012525-</t>
+        </is>
+      </c>
+      <c r="I29" s="25" t="inlineStr">
         <is>
           <t>P1208170-</t>
         </is>
       </c>
-      <c r="J29" s="14" t="n"/>
-      <c r="K29" s="22" t="inlineStr">
-        <is>
-          <t>b1004254-</t>
-        </is>
-      </c>
-      <c r="L29" s="22" t="inlineStr">
-        <is>
-          <t>M1016856-</t>
-        </is>
-      </c>
-      <c r="M29" s="22" t="inlineStr">
+      <c r="J29" s="25" t="inlineStr">
+        <is>
+          <t>T2003346-</t>
+        </is>
+      </c>
+      <c r="K29" s="25" t="inlineStr">
+        <is>
+          <t>M1016609-</t>
+        </is>
+      </c>
+      <c r="L29" s="25" t="inlineStr">
+        <is>
+          <t>B2011444-</t>
+        </is>
+      </c>
+      <c r="M29" s="25" t="inlineStr">
         <is>
           <t>m1009084-</t>
         </is>
       </c>
-      <c r="N29" s="22" t="inlineStr">
-        <is>
-          <t>B1004553-</t>
-        </is>
-      </c>
-      <c r="O29" s="14" t="n"/>
+      <c r="N29" s="25" t="inlineStr">
+        <is>
+          <t>B1008752-</t>
+        </is>
+      </c>
+      <c r="O29" s="25" t="inlineStr">
+        <is>
+          <t>B1005663-</t>
+        </is>
+      </c>
       <c r="P29" s="14" t="n"/>
-      <c r="Q29" s="14" t="n"/>
-      <c r="R29" s="14" t="n"/>
-      <c r="S29" s="22" t="inlineStr">
-        <is>
-          <t>B1005973-</t>
-        </is>
-      </c>
-      <c r="T29" s="22" t="inlineStr">
+      <c r="Q29" s="25" t="inlineStr">
+        <is>
+          <t>B1004853-</t>
+        </is>
+      </c>
+      <c r="R29" s="25" t="inlineStr">
+        <is>
+          <t>B1006945-</t>
+        </is>
+      </c>
+      <c r="S29" s="25" t="inlineStr">
+        <is>
+          <t>B2010623-</t>
+        </is>
+      </c>
+      <c r="T29" s="25" t="inlineStr">
         <is>
           <t>B1004824-</t>
         </is>
       </c>
-      <c r="U29" s="22" t="inlineStr">
-        <is>
-          <t>B2010656-</t>
-        </is>
-      </c>
-      <c r="V29" s="22" t="inlineStr">
-        <is>
-          <t>B2011065-</t>
-        </is>
-      </c>
-      <c r="W29" s="22" t="inlineStr">
+      <c r="U29" s="25" t="inlineStr">
+        <is>
+          <t>T2001332-</t>
+        </is>
+      </c>
+      <c r="V29" s="25" t="inlineStr">
+        <is>
+          <t>B2012330-</t>
+        </is>
+      </c>
+      <c r="W29" s="25" t="inlineStr">
         <is>
           <t>b2010462-</t>
         </is>
       </c>
-      <c r="X29" s="22" t="inlineStr">
-        <is>
-          <t>B2010925-</t>
-        </is>
-      </c>
-      <c r="Y29" s="22" t="inlineStr">
+      <c r="X29" s="25" t="inlineStr">
+        <is>
+          <t>B1008429-</t>
+        </is>
+      </c>
+      <c r="Y29" s="25" t="inlineStr">
         <is>
           <t>P1208896-</t>
         </is>
       </c>
-      <c r="Z29" s="14" t="n"/>
-      <c r="AA29" s="22" t="inlineStr">
+      <c r="Z29" s="25" t="inlineStr">
+        <is>
+          <t>b1006162-</t>
+        </is>
+      </c>
+      <c r="AA29" s="25" t="inlineStr">
         <is>
           <t>B1005051-</t>
         </is>
       </c>
-      <c r="AB29" s="22" t="inlineStr">
-        <is>
-          <t>b1008376-</t>
-        </is>
-      </c>
-      <c r="AC29" s="22" t="inlineStr">
+      <c r="AB29" s="25" t="inlineStr">
+        <is>
+          <t>B2010145-</t>
+        </is>
+      </c>
+      <c r="AC29" s="25" t="inlineStr">
         <is>
           <t>B2000049-</t>
         </is>
       </c>
-      <c r="AD29" s="14" t="n"/>
+      <c r="AD29" s="26" t="inlineStr">
+        <is>
+          <t>P1234133-
+T2002453-</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="17" t="n"/>
@@ -3819,21 +4016,33 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="21.5" customHeight="1" s="19">
+    <row r="31" ht="21.5" customHeight="1">
       <c r="A31" s="18" t="n"/>
       <c r="B31" s="16" t="n"/>
-      <c r="C31" s="23" t="inlineStr">
-        <is>
-          <t>b1006821-</t>
+      <c r="C31" s="27" t="inlineStr">
+        <is>
+          <t>B1004715-</t>
         </is>
       </c>
       <c r="D31" s="5" t="n"/>
       <c r="E31" s="5" t="n"/>
       <c r="F31" s="5" t="n"/>
-      <c r="G31" s="5" t="n"/>
+      <c r="G31" s="27" t="inlineStr">
+        <is>
+          <t>RW200479-</t>
+        </is>
+      </c>
       <c r="H31" s="5" t="n"/>
-      <c r="I31" s="5" t="n"/>
-      <c r="J31" s="5" t="n"/>
+      <c r="I31" s="27" t="inlineStr">
+        <is>
+          <t>B1004348-</t>
+        </is>
+      </c>
+      <c r="J31" s="27" t="inlineStr">
+        <is>
+          <t>B1004350-</t>
+        </is>
+      </c>
       <c r="K31" s="3" t="n"/>
       <c r="L31" s="3" t="n"/>
       <c r="M31" s="3" t="n"/>
@@ -3844,50 +4053,51 @@
       <c r="R31" s="3" t="n"/>
       <c r="S31" s="3" t="n"/>
       <c r="T31" s="3" t="n"/>
-      <c r="U31" s="3" t="n"/>
+      <c r="U31" s="27" t="inlineStr">
+        <is>
+          <t>B1005658-</t>
+        </is>
+      </c>
       <c r="V31" s="3" t="n"/>
-      <c r="W31" s="23" t="inlineStr">
-        <is>
-          <t>B1007269-</t>
-        </is>
-      </c>
-      <c r="X31" s="23" t="inlineStr">
-        <is>
-          <t>B1007271-</t>
-        </is>
-      </c>
-      <c r="Y31" s="23" t="inlineStr">
-        <is>
-          <t>b2010511-</t>
-        </is>
-      </c>
-      <c r="Z31" s="23" t="inlineStr">
-        <is>
-          <t>b1006162-</t>
-        </is>
-      </c>
-      <c r="AA31" s="23" t="inlineStr">
-        <is>
-          <t>B2010660-</t>
-        </is>
-      </c>
-      <c r="AB31" s="23" t="inlineStr">
-        <is>
-          <t>B2010465-</t>
-        </is>
-      </c>
-      <c r="AC31" s="23" t="inlineStr">
-        <is>
-          <t>P1201125-</t>
-        </is>
-      </c>
-      <c r="AD31" s="23" t="inlineStr">
-        <is>
-          <t>P1207123-</t>
+      <c r="W31" s="27" t="inlineStr">
+        <is>
+          <t>B2012221-</t>
+        </is>
+      </c>
+      <c r="X31" s="27" t="inlineStr">
+        <is>
+          <t>B2012227-</t>
+        </is>
+      </c>
+      <c r="Y31" s="28" t="inlineStr">
+        <is>
+          <t>B1008813-
+X1000222-</t>
+        </is>
+      </c>
+      <c r="Z31" s="27" t="inlineStr">
+        <is>
+          <t>B1004428-</t>
+        </is>
+      </c>
+      <c r="AA31" s="27" t="inlineStr">
+        <is>
+          <t>b2012284-</t>
+        </is>
+      </c>
+      <c r="AB31" s="3" t="n"/>
+      <c r="AC31" s="27" t="inlineStr">
+        <is>
+          <t>P1229817-</t>
+        </is>
+      </c>
+      <c r="AD31" s="27" t="inlineStr">
+        <is>
+          <t>B1004440-</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="21" customHeight="1" s="19">
+    <row r="32" ht="21" customHeight="1">
       <c r="A32" s="10" t="n"/>
       <c r="B32" s="10" t="n"/>
       <c r="C32" s="11" t="n"/>
@@ -3922,7 +4132,7 @@
     <row r="33"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A2:A15"/>
     <mergeCell ref="A18:A31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>